<commit_message>
Compressed script for RC and Modified other api's.
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/ENTITIES.xlsx
+++ b/Lexis-GLOBAL/Coredata/ENTITIES.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI_AdminPortal\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6092E8AD-2348-4621-83A1-A98AA271211E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F77BDF0-0C66-4EA5-A8BF-8BB74B9A3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,7 +534,8 @@
     <col min="11" max="11" width="17.36328125" customWidth="1"/>
     <col min="12" max="12" width="15.1796875" customWidth="1"/>
     <col min="13" max="13" width="13.7265625" customWidth="1"/>
-    <col min="14" max="16" width="8.7265625" customWidth="1"/>
+    <col min="14" max="14" width="17.453125" customWidth="1"/>
+    <col min="15" max="16" width="8.7265625" customWidth="1"/>
     <col min="17" max="17" width="20.81640625" customWidth="1"/>
     <col min="18" max="18" width="20.54296875" customWidth="1"/>
   </cols>

</xml_diff>